<commit_message>
update data on 21-07-22
</commit_message>
<xml_diff>
--- a/Python.xlsx
+++ b/Python.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Infos" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="152">
   <si>
     <t>https://www.youtube.com/watch?v=6DqMLtd7YIk&amp;list=PLAaOuSGREyM7t8kjTcxz7hx4bmVbdyjuV&amp;index=2</t>
   </si>
@@ -483,6 +483,12 @@
   </si>
   <si>
     <t>Cập nhật dữ liệu giao dịch PS hàng ngày để làm cơ sở phân tích (gồm bản FULL và Khớp lệnh)</t>
+  </si>
+  <si>
+    <t>Z</t>
+  </si>
+  <si>
+    <t>ghtD2389$rt</t>
   </si>
 </sst>
 </file>
@@ -1006,7 +1012,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
@@ -1129,10 +1135,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:C4"/>
+  <dimension ref="B2:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1159,6 +1165,14 @@
       </c>
       <c r="C4" t="s">
         <v>147</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B5" t="s">
+        <v>150</v>
+      </c>
+      <c r="C5" t="s">
+        <v>151</v>
       </c>
     </row>
   </sheetData>

</xml_diff>